<commit_message>
Updated plot taxanomy, added example datasets
</commit_message>
<xml_diff>
--- a/data/example_datasets/datasets_overview.xlsx
+++ b/data/example_datasets/datasets_overview.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -98,6 +98,33 @@
   </si>
   <si>
     <t xml:space="preserve">This data set consists of three types of entities: (a) the specification of an auto in terms of various characteristics, (b) its assigned insurance risk rating, (c) its normalized losses in use as compared to other cars. The second rating corresponds to the degree to which the auto is more risky than its price indicates. Cars are initially assigned a risk factor symbol associated with its price. Then, if it is more risky (or less), this symbol is adjusted by moving it up (or down) the scale. Actuarians call this process "symboling". A value of +3 indicates that the auto is risky, -3 that it is probably pretty safe. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kdd_cup_1998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.kdd.org/kdd-cup/view/kdd-cup-1998/Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is the data set used for The Second International Knowledge Discovery and Data Mining Tools Competition, which was held in conjunction with KDD-98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adult</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.kaggle.com/wenruliu/adult-income-dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An individual’s annual income results from various factors. Intuitively, it is influenced by the individual’s education level, age, gender, occupation, and etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">occupancy_detection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://archive.ics.uci.edu/ml/datasets/Occupancy+Detection+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It is a binary classification problem which requires that an observation of environmental factors such as temperature and humidity be used to classify whether a room is occupied or unoccupied. </t>
   </si>
 </sst>
 </file>
@@ -217,7 +244,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -252,6 +279,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -331,10 +362,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O5" activeCellId="0" sqref="O5"/>
+      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -588,6 +619,120 @@
         <v>0</v>
       </c>
     </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="9" t="n">
+        <v>191779</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>48842</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="J7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="M7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="N7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="O7" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="9" t="n">
+        <v>20560</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="J8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Updated dataset overview and added sp500 dataset
</commit_message>
<xml_diff>
--- a/data/example_datasets/datasets_overview.xlsx
+++ b/data/example_datasets/datasets_overview.xlsx
@@ -100,13 +100,13 @@
     <t xml:space="preserve">This data set consists of three types of entities: (a) the specification of an auto in terms of various characteristics, (b) its assigned insurance risk rating, (c) its normalized losses in use as compared to other cars. The second rating corresponds to the degree to which the auto is more risky than its price indicates. Cars are initially assigned a risk factor symbol associated with its price. Then, if it is more risky (or less), this symbol is adjusted by moving it up (or down) the scale. Actuarians call this process "symboling". A value of +3 indicates that the auto is risky, -3 that it is probably pretty safe. </t>
   </si>
   <si>
-    <t xml:space="preserve">kdd_cup_1998</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.kdd.org/kdd-cup/view/kdd-cup-1998/Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is the data set used for The Second International Knowledge Discovery and Data Mining Tools Competition, which was held in conjunction with KDD-98</t>
+    <t xml:space="preserve">sp500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.kaggle.com/camnugent/sandp500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stock market data can be interesting to analyze and as a further incentive, strong predictive models can have large financial payoff. The amount of financial data on the web is seemingly endless. A large and well structured dataset on a wide array of companies can be hard to come by. Here I provide a dataset with historical stock prices (last 5 years) for all companies currently found on the S&amp;P 500 index. </t>
   </si>
   <si>
     <t xml:space="preserve">adult</t>
@@ -365,7 +365,7 @@
   <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -633,10 +633,37 @@
         <v>28</v>
       </c>
       <c r="E6" s="9" t="n">
-        <v>191779</v>
+        <v>619404</v>
       </c>
       <c r="F6" s="1" t="n">
-        <v>481</v>
+        <v>7</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Updated dataset overview, added avocado prices dataset
</commit_message>
<xml_diff>
--- a/data/example_datasets/datasets_overview.xlsx
+++ b/data/example_datasets/datasets_overview.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -125,6 +125,15 @@
   </si>
   <si>
     <t xml:space="preserve">It is a binary classification problem which requires that an observation of environmental factors such as temperature and humidity be used to classify whether a room is occupied or unoccupied. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">avocado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.kaggle.com/neuromusic/avocado-prices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The table below represents weekly 2018 retail scan data for National retail volume (units) and price. Retail scan data comes directly from retailers’ cash registers based on actual retail sales of Hass avocados. Starting in 2013, the table below reflects an expanded, multi-outlet retail data set. Multi-outlet reporting includes an aggregation of the following channels: grocery, mass, club, drug, dollar and military. The Average Price (of avocados) in the table reflects a per unit (per avocado) cost, even when multiple units (avocados) are sold in bags. The Product Lookup codes (PLU’s) in the table are only for Hass avocados. Other varieties of avocados (e.g. greenskins) are not included in this table. </t>
   </si>
 </sst>
 </file>
@@ -362,10 +371,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:P1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -452,6 +461,7 @@
         <v>32</v>
       </c>
       <c r="F2" s="1" t="n">
+        <f aca="false">SUM(G2,L2)</f>
         <v>12</v>
       </c>
       <c r="G2" s="1" t="n">
@@ -461,7 +471,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="1" t="n">
-        <f aca="false">SUM(M2:N2)</f>
+        <f aca="false">SUM(M2:O2)</f>
         <v>1</v>
       </c>
       <c r="M2" s="1" t="n">
@@ -489,10 +499,11 @@
         <v>142</v>
       </c>
       <c r="F3" s="1" t="n">
+        <f aca="false">SUM(G3,L3)</f>
         <v>5</v>
       </c>
       <c r="G3" s="1" t="n">
-        <f aca="false">SUM(I3:K3)</f>
+        <f aca="false">SUM(H3:K3)</f>
         <v>3</v>
       </c>
       <c r="H3" s="1" t="n">
@@ -508,7 +519,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="1" t="n">
-        <f aca="false">SUM(M3:N3)</f>
+        <f aca="false">SUM(M3:O3)</f>
         <v>2</v>
       </c>
       <c r="M3" s="1" t="n">
@@ -539,10 +550,11 @@
         <v>7043</v>
       </c>
       <c r="F4" s="1" t="n">
+        <f aca="false">SUM(G4,L4)</f>
         <v>21</v>
       </c>
       <c r="G4" s="1" t="n">
-        <f aca="false">SUM(I4:K4)</f>
+        <f aca="false">SUM(H4:K4)</f>
         <v>4</v>
       </c>
       <c r="H4" s="1" t="n">
@@ -558,8 +570,8 @@
         <v>1</v>
       </c>
       <c r="L4" s="1" t="n">
-        <f aca="false">SUM(M4:N4)</f>
-        <v>12</v>
+        <f aca="false">SUM(M4:O4)</f>
+        <v>17</v>
       </c>
       <c r="M4" s="1" t="n">
         <v>1</v>
@@ -589,9 +601,11 @@
         <v>205</v>
       </c>
       <c r="F5" s="1" t="n">
+        <f aca="false">SUM(G5,L5)</f>
         <v>26</v>
       </c>
       <c r="G5" s="1" t="n">
+        <f aca="false">SUM(H5:K5)</f>
         <v>16</v>
       </c>
       <c r="H5" s="1" t="n">
@@ -607,6 +621,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="1" t="n">
+        <f aca="false">SUM(M5:O5)</f>
         <v>10</v>
       </c>
       <c r="M5" s="1" t="n">
@@ -636,10 +651,12 @@
         <v>619404</v>
       </c>
       <c r="F6" s="1" t="n">
+        <f aca="false">SUM(G6,L6)</f>
         <v>7</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>0</v>
+        <f aca="false">SUM(H6:K6)</f>
+        <v>6</v>
       </c>
       <c r="H6" s="1" t="n">
         <v>1</v>
@@ -654,13 +671,14 @@
         <v>0</v>
       </c>
       <c r="L6" s="1" t="n">
+        <f aca="false">SUM(M6:O6)</f>
         <v>1</v>
       </c>
       <c r="M6" s="1" t="n">
         <v>0</v>
       </c>
       <c r="N6" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6" s="1" t="n">
         <v>0</v>
@@ -683,9 +701,11 @@
         <v>48842</v>
       </c>
       <c r="F7" s="1" t="n">
+        <f aca="false">SUM(G7,L7)</f>
         <v>15</v>
       </c>
       <c r="G7" s="1" t="n">
+        <f aca="false">SUM(H7:K7)</f>
         <v>7</v>
       </c>
       <c r="H7" s="1" t="n">
@@ -701,6 +721,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="1" t="n">
+        <f aca="false">SUM(M7:O7)</f>
         <v>8</v>
       </c>
       <c r="M7" s="1" t="n">
@@ -730,36 +751,90 @@
         <v>20560</v>
       </c>
       <c r="F8" s="1" t="n">
+        <f aca="false">SUM(G8,L8)</f>
         <v>7</v>
       </c>
       <c r="G8" s="1" t="n">
+        <f aca="false">SUM(H8:K8)</f>
         <v>7</v>
       </c>
       <c r="H8" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I8" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="J8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" s="1" t="n">
+        <f aca="false">SUM(M8:O8)</f>
+        <v>0</v>
+      </c>
+      <c r="M8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>18250</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <f aca="false">SUM(G9,L9)</f>
+        <v>14</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <f aca="false">SUM(H9:K9)</f>
+        <v>12</v>
+      </c>
+      <c r="H9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="J8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="K8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O8" s="1" t="n">
+      <c r="J9" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="K9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1" t="n">
+        <f aca="false">SUM(M9:O9)</f>
+        <v>2</v>
+      </c>
+      <c r="M9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="O9" s="1" t="n">
         <v>0</v>
       </c>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>